<commit_message>
switched LS and HS outputs to match hardware timers distribution. Added a 2k pulldown for the tach output"
</commit_message>
<xml_diff>
--- a/export/V0.1/hw_proteus_72_CPL.xlsx
+++ b/export/V0.1/hw_proteus_72_CPL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\RUSEFI\PnPRE\PROTEUS\hw_proteus_72_NB\export\V0.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\RUSEFI\Gits\hw_PnProteus_72P_NB2\export\V0.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F632FCB-B534-4DFE-98B1-671B6E5C84C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF538FCD-0E26-46DB-93BE-30905ED5C6F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="6585" windowWidth="21600" windowHeight="8970"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hw_proteus_72_NB-all-pos" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="129">
   <si>
     <t>D1</t>
   </si>
@@ -404,12 +404,15 @@
   </si>
   <si>
     <t>Rotation</t>
+  </si>
+  <si>
+    <t>R17</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1243,11 +1246,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E123"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E124"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2121,27 +2124,27 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
       <c r="B52">
-        <v>118.184</v>
+        <v>118.2</v>
       </c>
       <c r="C52">
-        <v>-117.137</v>
+        <v>-87.5</v>
       </c>
       <c r="D52" t="s">
         <v>1</v>
       </c>
       <c r="E52">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53">
-        <v>120.75700000000001</v>
+        <v>118.184</v>
       </c>
       <c r="C53">
         <v>-117.137</v>
@@ -2155,44 +2158,44 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54">
-        <v>138.30000000000001</v>
+        <v>120.75700000000001</v>
       </c>
       <c r="C54">
-        <v>-105.607</v>
+        <v>-117.137</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55">
-        <v>123.33</v>
+        <v>138.30000000000001</v>
       </c>
       <c r="C55">
-        <v>-117.137</v>
+        <v>-105.607</v>
       </c>
       <c r="D55" t="s">
         <v>1</v>
       </c>
       <c r="E55">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56">
-        <v>125.90300000000001</v>
+        <v>123.33</v>
       </c>
       <c r="C56">
         <v>-117.137</v>
@@ -2206,44 +2209,44 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57">
-        <v>138.30000000000001</v>
+        <v>125.90300000000001</v>
       </c>
       <c r="C57">
-        <v>-103.063</v>
+        <v>-117.137</v>
       </c>
       <c r="D57" t="s">
         <v>1</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58">
-        <v>128.47499999999999</v>
+        <v>138.30000000000001</v>
       </c>
       <c r="C58">
-        <v>-117.137</v>
+        <v>-103.063</v>
       </c>
       <c r="D58" t="s">
         <v>1</v>
       </c>
       <c r="E58">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59">
-        <v>131.048</v>
+        <v>128.47499999999999</v>
       </c>
       <c r="C59">
         <v>-117.137</v>
@@ -2257,44 +2260,44 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60">
-        <v>138.30000000000001</v>
+        <v>131.048</v>
       </c>
       <c r="C60">
-        <v>-100.51900000000001</v>
+        <v>-117.137</v>
       </c>
       <c r="D60" t="s">
         <v>1</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61">
-        <v>133.62100000000001</v>
+        <v>138.30000000000001</v>
       </c>
       <c r="C61">
-        <v>-117.137</v>
+        <v>-100.51900000000001</v>
       </c>
       <c r="D61" t="s">
         <v>1</v>
       </c>
       <c r="E61">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62">
-        <v>136.19399999999999</v>
+        <v>133.62100000000001</v>
       </c>
       <c r="C62">
         <v>-117.137</v>
@@ -2308,10 +2311,10 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63">
-        <v>138.767</v>
+        <v>136.19399999999999</v>
       </c>
       <c r="C63">
         <v>-117.137</v>
@@ -2325,10 +2328,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64">
-        <v>141.34</v>
+        <v>138.767</v>
       </c>
       <c r="C64">
         <v>-117.137</v>
@@ -2342,44 +2345,44 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65">
-        <v>138.30000000000001</v>
+        <v>141.34</v>
       </c>
       <c r="C65">
-        <v>-97.974800000000002</v>
+        <v>-117.137</v>
       </c>
       <c r="D65" t="s">
         <v>1</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66">
-        <v>143.91300000000001</v>
+        <v>138.30000000000001</v>
       </c>
       <c r="C66">
-        <v>-117.137</v>
+        <v>-97.974800000000002</v>
       </c>
       <c r="D66" t="s">
         <v>1</v>
       </c>
       <c r="E66">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67">
-        <v>146.48599999999999</v>
+        <v>143.91300000000001</v>
       </c>
       <c r="C67">
         <v>-117.137</v>
@@ -2393,44 +2396,44 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68">
-        <v>138.30000000000001</v>
+        <v>146.48599999999999</v>
       </c>
       <c r="C68">
-        <v>-95.430800000000005</v>
+        <v>-117.137</v>
       </c>
       <c r="D68" t="s">
         <v>1</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69">
-        <v>149.059</v>
+        <v>138.30000000000001</v>
       </c>
       <c r="C69">
-        <v>-117.137</v>
+        <v>-95.430800000000005</v>
       </c>
       <c r="D69" t="s">
         <v>1</v>
       </c>
       <c r="E69">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70">
-        <v>151.63200000000001</v>
+        <v>149.059</v>
       </c>
       <c r="C70">
         <v>-117.137</v>
@@ -2444,44 +2447,44 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71">
-        <v>138.30000000000001</v>
+        <v>151.63200000000001</v>
       </c>
       <c r="C71">
-        <v>-92.886799999999994</v>
+        <v>-117.137</v>
       </c>
       <c r="D71" t="s">
         <v>1</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72">
-        <v>154.20500000000001</v>
+        <v>138.30000000000001</v>
       </c>
       <c r="C72">
-        <v>-117.137</v>
+        <v>-92.886799999999994</v>
       </c>
       <c r="D72" t="s">
         <v>1</v>
       </c>
       <c r="E72">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73">
-        <v>156.77799999999999</v>
+        <v>154.20500000000001</v>
       </c>
       <c r="C73">
         <v>-117.137</v>
@@ -2495,78 +2498,78 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74">
-        <v>124.54</v>
+        <v>156.77799999999999</v>
       </c>
       <c r="C74">
-        <v>-95.066800000000001</v>
+        <v>-117.137</v>
       </c>
       <c r="D74" t="s">
         <v>1</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75">
-        <v>159.35</v>
+        <v>124.54</v>
       </c>
       <c r="C75">
-        <v>-117.137</v>
+        <v>-95.066800000000001</v>
       </c>
       <c r="D75" t="s">
         <v>1</v>
       </c>
       <c r="E75">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76">
-        <v>124.54</v>
+        <v>159.35</v>
       </c>
       <c r="C76">
-        <v>-92.522800000000004</v>
+        <v>-117.137</v>
       </c>
       <c r="D76" t="s">
         <v>1</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77">
-        <v>161.923</v>
+        <v>124.54</v>
       </c>
       <c r="C77">
-        <v>-117.137</v>
+        <v>-92.522800000000004</v>
       </c>
       <c r="D77" t="s">
         <v>1</v>
       </c>
       <c r="E77">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78">
-        <v>164.49600000000001</v>
+        <v>161.923</v>
       </c>
       <c r="C78">
         <v>-117.137</v>
@@ -2580,44 +2583,44 @@
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79">
-        <v>124.54</v>
+        <v>164.49600000000001</v>
       </c>
       <c r="C79">
-        <v>-89.978800000000007</v>
+        <v>-117.137</v>
       </c>
       <c r="D79" t="s">
         <v>1</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80">
-        <v>167.06899999999999</v>
+        <v>124.54</v>
       </c>
       <c r="C80">
-        <v>-117.137</v>
+        <v>-89.978800000000007</v>
       </c>
       <c r="D80" t="s">
         <v>1</v>
       </c>
       <c r="E80">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81">
-        <v>169.642</v>
+        <v>167.06899999999999</v>
       </c>
       <c r="C81">
         <v>-117.137</v>
@@ -2631,44 +2634,44 @@
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82">
-        <v>124.54</v>
+        <v>169.642</v>
       </c>
       <c r="C82">
-        <v>-87.434799999999996</v>
+        <v>-117.137</v>
       </c>
       <c r="D82" t="s">
         <v>1</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83">
-        <v>172.215</v>
+        <v>124.54</v>
       </c>
       <c r="C83">
-        <v>-117.137</v>
+        <v>-87.434799999999996</v>
       </c>
       <c r="D83" t="s">
         <v>1</v>
       </c>
       <c r="E83">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84">
-        <v>174.78800000000001</v>
+        <v>172.215</v>
       </c>
       <c r="C84">
         <v>-117.137</v>
@@ -2682,10 +2685,10 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B85">
-        <v>177.36099999999999</v>
+        <v>174.78800000000001</v>
       </c>
       <c r="C85">
         <v>-117.137</v>
@@ -2699,44 +2702,44 @@
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86">
-        <v>124.54</v>
+        <v>177.36099999999999</v>
       </c>
       <c r="C86">
-        <v>-85.017799999999994</v>
+        <v>-117.137</v>
       </c>
       <c r="D86" t="s">
         <v>1</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B87">
-        <v>179.934</v>
+        <v>124.54</v>
       </c>
       <c r="C87">
-        <v>-117.137</v>
+        <v>-85.017799999999994</v>
       </c>
       <c r="D87" t="s">
         <v>1</v>
       </c>
       <c r="E87">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B88">
-        <v>182.50700000000001</v>
+        <v>179.934</v>
       </c>
       <c r="C88">
         <v>-117.137</v>
@@ -2750,44 +2753,44 @@
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89">
-        <v>124.54</v>
+        <v>182.50700000000001</v>
       </c>
       <c r="C89">
-        <v>-82.346800000000002</v>
+        <v>-117.137</v>
       </c>
       <c r="D89" t="s">
         <v>1</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B90">
-        <v>185.08</v>
+        <v>124.54</v>
       </c>
       <c r="C90">
-        <v>-117.137</v>
+        <v>-82.346800000000002</v>
       </c>
       <c r="D90" t="s">
         <v>1</v>
       </c>
       <c r="E90">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91">
-        <v>187.65299999999999</v>
+        <v>185.08</v>
       </c>
       <c r="C91">
         <v>-117.137</v>
@@ -2801,44 +2804,44 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B92">
-        <v>138.22</v>
+        <v>187.65299999999999</v>
       </c>
       <c r="C92">
-        <v>-86.336799999999997</v>
+        <v>-117.137</v>
       </c>
       <c r="D92" t="s">
         <v>1</v>
       </c>
       <c r="E92">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93">
-        <v>190.22499999999999</v>
+        <v>138.22</v>
       </c>
       <c r="C93">
-        <v>-117.137</v>
+        <v>-86.336799999999997</v>
       </c>
       <c r="D93" t="s">
         <v>1</v>
       </c>
       <c r="E93">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B94">
-        <v>192.798</v>
+        <v>190.22499999999999</v>
       </c>
       <c r="C94">
         <v>-117.137</v>
@@ -2852,44 +2855,44 @@
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95">
-        <v>240.04499999999999</v>
+        <v>192.798</v>
       </c>
       <c r="C95">
-        <v>-81.9268</v>
+        <v>-117.137</v>
       </c>
       <c r="D95" t="s">
         <v>1</v>
       </c>
       <c r="E95">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B96">
-        <v>195.37100000000001</v>
+        <v>240.04499999999999</v>
       </c>
       <c r="C96">
-        <v>-117.137</v>
+        <v>-81.9268</v>
       </c>
       <c r="D96" t="s">
         <v>1</v>
       </c>
       <c r="E96">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B97">
-        <v>197.94399999999999</v>
+        <v>195.37100000000001</v>
       </c>
       <c r="C97">
         <v>-117.137</v>
@@ -2903,112 +2906,112 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B98">
-        <v>240.22</v>
+        <v>197.94399999999999</v>
       </c>
       <c r="C98">
-        <v>-84.510099999999994</v>
+        <v>-117.137</v>
       </c>
       <c r="D98" t="s">
         <v>1</v>
       </c>
       <c r="E98">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B99">
-        <v>200.517</v>
+        <v>240.22</v>
       </c>
       <c r="C99">
-        <v>-117.137</v>
+        <v>-84.510099999999994</v>
       </c>
       <c r="D99" t="s">
         <v>1</v>
       </c>
       <c r="E99">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B100">
-        <v>240.065</v>
+        <v>200.517</v>
       </c>
       <c r="C100">
-        <v>-87.093500000000006</v>
+        <v>-117.137</v>
       </c>
       <c r="D100" t="s">
         <v>1</v>
       </c>
       <c r="E100">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B101">
-        <v>203.09</v>
+        <v>240.065</v>
       </c>
       <c r="C101">
-        <v>-117.137</v>
+        <v>-87.093500000000006</v>
       </c>
       <c r="D101" t="s">
         <v>1</v>
       </c>
       <c r="E101">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B102">
-        <v>240.04499999999999</v>
+        <v>203.09</v>
       </c>
       <c r="C102">
-        <v>-89.6768</v>
+        <v>-117.137</v>
       </c>
       <c r="D102" t="s">
         <v>1</v>
       </c>
       <c r="E102">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B103">
-        <v>205.66300000000001</v>
+        <v>240.04499999999999</v>
       </c>
       <c r="C103">
-        <v>-117.137</v>
+        <v>-89.6768</v>
       </c>
       <c r="D103" t="s">
         <v>1</v>
       </c>
       <c r="E103">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B104">
-        <v>210.809</v>
+        <v>205.66300000000001</v>
       </c>
       <c r="C104">
         <v>-117.137</v>
@@ -3022,44 +3025,44 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B105">
-        <v>240.04499999999999</v>
+        <v>210.809</v>
       </c>
       <c r="C105">
-        <v>-92.260099999999994</v>
+        <v>-117.137</v>
       </c>
       <c r="D105" t="s">
         <v>1</v>
       </c>
       <c r="E105">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B106">
-        <v>208.23599999999999</v>
+        <v>240.04499999999999</v>
       </c>
       <c r="C106">
-        <v>-117.137</v>
+        <v>-92.260099999999994</v>
       </c>
       <c r="D106" t="s">
         <v>1</v>
       </c>
       <c r="E106">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B107">
-        <v>213.38200000000001</v>
+        <v>208.23599999999999</v>
       </c>
       <c r="C107">
         <v>-117.137</v>
@@ -3073,10 +3076,10 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B108">
-        <v>215.95500000000001</v>
+        <v>213.38200000000001</v>
       </c>
       <c r="C108">
         <v>-117.137</v>
@@ -3090,10 +3093,10 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B109">
-        <v>218.52799999999999</v>
+        <v>215.95500000000001</v>
       </c>
       <c r="C109">
         <v>-117.137</v>
@@ -3107,44 +3110,44 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B110">
-        <v>240.01499999999999</v>
+        <v>218.52799999999999</v>
       </c>
       <c r="C110">
-        <v>-94.843500000000006</v>
+        <v>-117.137</v>
       </c>
       <c r="D110" t="s">
         <v>1</v>
       </c>
       <c r="E110">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B111">
-        <v>221.1</v>
+        <v>240.01499999999999</v>
       </c>
       <c r="C111">
-        <v>-117.137</v>
+        <v>-94.843500000000006</v>
       </c>
       <c r="D111" t="s">
         <v>1</v>
       </c>
       <c r="E111">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B112">
-        <v>223.673</v>
+        <v>221.1</v>
       </c>
       <c r="C112">
         <v>-117.137</v>
@@ -3158,44 +3161,44 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B113">
-        <v>240.01499999999999</v>
+        <v>223.673</v>
       </c>
       <c r="C113">
-        <v>-97.4268</v>
+        <v>-117.137</v>
       </c>
       <c r="D113" t="s">
         <v>1</v>
       </c>
       <c r="E113">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B114">
-        <v>226.24600000000001</v>
+        <v>240.01499999999999</v>
       </c>
       <c r="C114">
-        <v>-117.137</v>
+        <v>-97.4268</v>
       </c>
       <c r="D114" t="s">
         <v>1</v>
       </c>
       <c r="E114">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B115">
-        <v>228.81899999999999</v>
+        <v>226.24600000000001</v>
       </c>
       <c r="C115">
         <v>-117.137</v>
@@ -3209,10 +3212,10 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B116">
-        <v>231.392</v>
+        <v>228.81899999999999</v>
       </c>
       <c r="C116">
         <v>-117.137</v>
@@ -3226,10 +3229,10 @@
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B117">
-        <v>233.965</v>
+        <v>231.392</v>
       </c>
       <c r="C117">
         <v>-117.137</v>
@@ -3243,78 +3246,78 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B118">
-        <v>240.01499999999999</v>
+        <v>233.965</v>
       </c>
       <c r="C118">
-        <v>-100.01</v>
+        <v>-117.137</v>
       </c>
       <c r="D118" t="s">
         <v>1</v>
       </c>
       <c r="E118">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B119">
-        <v>236.53800000000001</v>
+        <v>240.01499999999999</v>
       </c>
       <c r="C119">
-        <v>-117.137</v>
+        <v>-100.01</v>
       </c>
       <c r="D119" t="s">
         <v>1</v>
       </c>
       <c r="E119">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B120">
-        <v>240.01499999999999</v>
+        <v>236.53800000000001</v>
       </c>
       <c r="C120">
-        <v>-102.593</v>
+        <v>-117.137</v>
       </c>
       <c r="D120" t="s">
         <v>1</v>
       </c>
       <c r="E120">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B121">
-        <v>239.11099999999999</v>
+        <v>240.01499999999999</v>
       </c>
       <c r="C121">
-        <v>-117.137</v>
+        <v>-102.593</v>
       </c>
       <c r="D121" t="s">
         <v>1</v>
       </c>
       <c r="E121">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B122">
-        <v>241.684</v>
+        <v>239.11099999999999</v>
       </c>
       <c r="C122">
         <v>-117.137</v>
@@ -3328,18 +3331,35 @@
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>121</v>
+      </c>
+      <c r="B123">
+        <v>241.684</v>
+      </c>
+      <c r="C123">
+        <v>-117.137</v>
+      </c>
+      <c r="D123" t="s">
+        <v>1</v>
+      </c>
+      <c r="E123">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>122</v>
       </c>
-      <c r="B123">
+      <c r="B124">
         <v>240.01499999999999</v>
       </c>
-      <c r="C123">
+      <c r="C124">
         <v>-105.17700000000001</v>
       </c>
-      <c r="D123" t="s">
-        <v>1</v>
-      </c>
-      <c r="E123">
+      <c r="D124" t="s">
+        <v>1</v>
+      </c>
+      <c r="E124">
         <v>180</v>
       </c>
     </row>

</xml_diff>